<commit_message>
added features and new flow
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konag\Desktop\aihrmsv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB45262B-8E5F-49F0-B3D1-30EEA33A63B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3624EC11-D900-447C-835E-6D22F292A93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,10 +145,10 @@
     <t>+919381879740</t>
   </si>
   <si>
-    <t>+919553566882</t>
-  </si>
-  <si>
     <t>+919493362006</t>
+  </si>
+  <si>
+    <t>+919110790210</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1413,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1537,7 +1537,7 @@
         <v>29</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1566,7 +1566,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>